<commit_message>
add selection de visualización
</commit_message>
<xml_diff>
--- a/src/assets/data/excel.xlsx
+++ b/src/assets/data/excel.xlsx
@@ -78,12 +78,6 @@
     <t>Posición</t>
   </si>
   <si>
-    <t>salto lugares</t>
-  </si>
-  <si>
-    <t>clase</t>
-  </si>
-  <si>
     <t>Akateko</t>
   </si>
   <si>
@@ -586,6 +580,12 @@
   </si>
   <si>
     <t>Zo</t>
+  </si>
+  <si>
+    <t>Posición en la tabla periódica</t>
+  </si>
+  <si>
+    <t>Clase html</t>
   </si>
 </sst>
 </file>
@@ -734,7 +734,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -757,6 +757,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1152,8 +1153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:U1048576"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1203,7 +1204,7 @@
       <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="20" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="4" t="s">
@@ -1237,10 +1238,10 @@
         <v>16</v>
       </c>
       <c r="S1" t="s">
-        <v>17</v>
+        <v>185</v>
       </c>
       <c r="T1" t="s">
-        <v>18</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:21">
@@ -1248,16 +1249,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>20</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>22</v>
       </c>
       <c r="F2" s="8">
         <v>3202</v>
@@ -1293,7 +1294,7 @@
         <v>0.91675119368361502</v>
       </c>
       <c r="Q2" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="R2">
         <v>25</v>
@@ -1302,7 +1303,7 @@
         <v>0</v>
       </c>
       <c r="T2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -1310,16 +1311,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="E3" s="8" t="s">
         <v>26</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="F3" s="8">
         <v>75953</v>
@@ -1355,7 +1356,7 @@
         <v>0.94809251023330898</v>
       </c>
       <c r="Q3" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="R3">
         <v>18</v>
@@ -1364,7 +1365,7 @@
         <v>0</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:21">
@@ -1372,16 +1373,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F4" s="8">
         <v>31</v>
@@ -1417,7 +1418,7 @@
         <v>2.8066959628016002</v>
       </c>
       <c r="Q4" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="R4">
         <v>26</v>
@@ -1426,7 +1427,7 @@
         <v>0</v>
       </c>
       <c r="T4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:21">
@@ -1434,16 +1435,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="E5" s="8" t="s">
         <v>34</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>36</v>
       </c>
       <c r="F5" s="8">
         <v>35</v>
@@ -1479,7 +1480,7 @@
         <v>1.47012441700757</v>
       </c>
       <c r="Q5" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="R5">
         <v>4</v>
@@ -1488,7 +1489,7 @@
         <v>14</v>
       </c>
       <c r="T5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="U5"/>
     </row>
@@ -1497,16 +1498,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="E6" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>42</v>
       </c>
       <c r="F6" s="8">
         <v>37300</v>
@@ -1542,7 +1543,7 @@
         <v>1.5401790701593401</v>
       </c>
       <c r="Q6" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="R6">
         <v>15</v>
@@ -1551,7 +1552,7 @@
         <v>0</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -1559,16 +1560,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="E7" s="8" t="s">
         <v>45</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>47</v>
       </c>
       <c r="F7" s="8">
         <v>542</v>
@@ -1604,7 +1605,7 @@
         <v>0.17428033177742799</v>
       </c>
       <c r="Q7" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="R7">
         <v>2</v>
@@ -1613,7 +1614,7 @@
         <v>0</v>
       </c>
       <c r="T7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -1621,16 +1622,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F8" s="8">
         <v>22086</v>
@@ -1666,7 +1667,7 @@
         <v>0.52971348845539601</v>
       </c>
       <c r="Q8" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="R8">
         <v>23</v>
@@ -1675,7 +1676,7 @@
         <v>0</v>
       </c>
       <c r="T8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:21">
@@ -1683,16 +1684,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F9" s="8">
         <v>69663</v>
@@ -1728,7 +1729,7 @@
         <v>1.1978960440968001</v>
       </c>
       <c r="Q9" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="R9">
         <v>19</v>
@@ -1737,7 +1738,7 @@
         <v>0</v>
       </c>
       <c r="T9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:21">
@@ -1745,16 +1746,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F10" s="8">
         <v>4709</v>
@@ -1790,7 +1791,7 @@
         <v>0.82750050846985401</v>
       </c>
       <c r="Q10" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="R10">
         <v>20</v>
@@ -1799,7 +1800,7 @@
         <v>0</v>
       </c>
       <c r="T10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -1807,16 +1808,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F11" s="8">
         <v>211760</v>
@@ -1852,7 +1853,7 @@
         <v>0.730684018685965</v>
       </c>
       <c r="Q11" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="R11">
         <v>21</v>
@@ -1861,7 +1862,7 @@
         <v>0</v>
       </c>
       <c r="T11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:21">
@@ -1869,16 +1870,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F12" s="8">
         <v>1296</v>
@@ -1914,7 +1915,7 @@
         <v>1.50600810425719</v>
       </c>
       <c r="Q12" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="R12">
         <v>22</v>
@@ -1923,7 +1924,7 @@
         <v>0</v>
       </c>
       <c r="T12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:21">
@@ -1931,16 +1932,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>61</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>63</v>
       </c>
       <c r="F13" s="8">
         <v>10848</v>
@@ -1976,7 +1977,7 @@
         <v>0.33041961516653101</v>
       </c>
       <c r="Q13" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="R13">
         <v>24</v>
@@ -1985,7 +1986,7 @@
         <v>0</v>
       </c>
       <c r="T13" s="13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:21">
@@ -1993,16 +1994,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F14" s="8">
         <v>57792</v>
@@ -2038,7 +2039,7 @@
         <v>0.35325693606807701</v>
       </c>
       <c r="Q14" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="R14">
         <v>27</v>
@@ -2047,7 +2048,7 @@
         <v>0</v>
       </c>
       <c r="T14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -2055,16 +2056,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F15" s="8">
         <v>4557</v>
@@ -2100,7 +2101,7 @@
         <v>1.1296032198328601</v>
       </c>
       <c r="Q15" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="R15">
         <v>28</v>
@@ -2109,7 +2110,7 @@
         <v>0</v>
       </c>
       <c r="T15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:21">
@@ -2117,16 +2118,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F16" s="8">
         <v>328867</v>
@@ -2162,7 +2163,7 @@
         <v>1.0469456460717299</v>
       </c>
       <c r="Q16" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="R16">
         <v>29</v>
@@ -2171,7 +2172,7 @@
         <v>0</v>
       </c>
       <c r="T16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:20">
@@ -2179,16 +2180,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F17" s="8">
         <v>2946</v>
@@ -2224,7 +2225,7 @@
         <v>0.97916940978882006</v>
       </c>
       <c r="Q17" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="R17">
         <v>16</v>
@@ -2233,7 +2234,7 @@
         <v>0</v>
       </c>
       <c r="T17" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:20">
@@ -2241,16 +2242,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F18" s="8">
         <v>255190</v>
@@ -2286,7 +2287,7 @@
         <v>0.85611327694612505</v>
       </c>
       <c r="Q18" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="R18">
         <v>41</v>
@@ -2295,7 +2296,7 @@
         <v>0</v>
       </c>
       <c r="T18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:20">
@@ -2303,16 +2304,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E19" s="8" t="s">
         <v>75</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>77</v>
       </c>
       <c r="F19" s="8">
         <v>24222</v>
@@ -2348,7 +2349,7 @@
         <v>0.97190862200896899</v>
       </c>
       <c r="Q19" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="R19">
         <v>40</v>
@@ -2357,7 +2358,7 @@
         <v>0</v>
       </c>
       <c r="T19" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:20">
@@ -2365,16 +2366,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F20" s="8">
         <v>71450</v>
@@ -2410,7 +2411,7 @@
         <v>1.3124762390784099</v>
       </c>
       <c r="Q20" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="R20">
         <v>17</v>
@@ -2419,7 +2420,7 @@
         <v>0</v>
       </c>
       <c r="T20" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:20">
@@ -2427,16 +2428,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F21" s="8">
         <v>485</v>
@@ -2472,7 +2473,7 @@
         <v>0.51571235946967198</v>
       </c>
       <c r="Q21" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="R21">
         <v>34</v>
@@ -2481,7 +2482,7 @@
         <v>0</v>
       </c>
       <c r="T21" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:20">
@@ -2489,16 +2490,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F22" s="8">
         <v>335</v>
@@ -2534,7 +2535,7 @@
         <v>0</v>
       </c>
       <c r="Q22" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="R22">
         <v>42</v>
@@ -2543,7 +2544,7 @@
         <v>0</v>
       </c>
       <c r="T22" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:20">
@@ -2551,16 +2552,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F23" s="8">
         <v>1315</v>
@@ -2596,7 +2597,7 @@
         <v>0.50561002451293102</v>
       </c>
       <c r="Q23" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="R23">
         <v>43</v>
@@ -2605,7 +2606,7 @@
         <v>0</v>
       </c>
       <c r="T23" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:20">
@@ -2613,16 +2614,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F24" s="8">
         <v>207</v>
@@ -2658,7 +2659,7 @@
         <v>0</v>
       </c>
       <c r="Q24" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="R24">
         <v>44</v>
@@ -2667,7 +2668,7 @@
         <v>0</v>
       </c>
       <c r="T24" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:20">
@@ -2675,16 +2676,16 @@
         <v>24</v>
       </c>
       <c r="B25" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D25" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="E25" s="8" t="s">
         <v>90</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>92</v>
       </c>
       <c r="F25" s="8">
         <v>241</v>
@@ -2720,7 +2721,7 @@
         <v>0.154119653326457</v>
       </c>
       <c r="Q25" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="R25">
         <v>1</v>
@@ -2729,7 +2730,7 @@
         <v>0</v>
       </c>
       <c r="T25" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:20">
@@ -2737,16 +2738,16 @@
         <v>25</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F26" s="8">
         <v>306</v>
@@ -2782,7 +2783,7 @@
         <v>0.27672930202495399</v>
       </c>
       <c r="Q26" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="R26">
         <v>3</v>
@@ -2791,7 +2792,7 @@
         <v>0</v>
       </c>
       <c r="T26" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:20">
@@ -2799,16 +2800,16 @@
         <v>26</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F27" s="8">
         <v>1197</v>
@@ -2844,7 +2845,7 @@
         <v>1.5458780270106001</v>
       </c>
       <c r="Q27" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="R27">
         <v>7</v>
@@ -2853,7 +2854,7 @@
         <v>0</v>
       </c>
       <c r="T27" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:20">
@@ -2861,16 +2862,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F28" s="8"/>
       <c r="G28" s="8"/>
@@ -2891,7 +2892,7 @@
         <v>0</v>
       </c>
       <c r="T28" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:20">
@@ -2899,16 +2900,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F29" s="8">
         <v>1388</v>
@@ -2944,7 +2945,7 @@
         <v>0.773362034232004</v>
       </c>
       <c r="Q29" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="R29">
         <v>45</v>
@@ -2953,7 +2954,7 @@
         <v>0</v>
       </c>
       <c r="T29" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:20">
@@ -2961,16 +2962,16 @@
         <v>29</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F30" s="8">
         <v>1166</v>
@@ -3006,7 +3007,7 @@
         <v>1.08928601546321</v>
       </c>
       <c r="Q30" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="R30">
         <v>57</v>
@@ -3015,7 +3016,7 @@
         <v>0</v>
       </c>
       <c r="T30" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:20">
@@ -3023,16 +3024,16 @@
         <v>30</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F31" s="8">
         <v>27050</v>
@@ -3068,7 +3069,7 @@
         <v>0.26566922565156897</v>
       </c>
       <c r="Q31" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="R31">
         <v>58</v>
@@ -3077,7 +3078,7 @@
         <v>0</v>
       </c>
       <c r="T31" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:20">
@@ -3085,16 +3086,16 @@
         <v>31</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F32" s="8">
         <v>3893</v>
@@ -3130,7 +3131,7 @@
         <v>0.174094052412962</v>
       </c>
       <c r="Q32" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="R32">
         <v>35</v>
@@ -3139,7 +3140,7 @@
         <v>0</v>
       </c>
       <c r="T32" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:21">
@@ -3147,16 +3148,16 @@
         <v>32</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F33" s="8">
         <v>1646782</v>
@@ -3192,7 +3193,7 @@
         <v>0.348721993979769</v>
       </c>
       <c r="Q33" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="R33">
         <v>59</v>
@@ -3201,7 +3202,7 @@
         <v>0</v>
       </c>
       <c r="T33" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:21">
@@ -3209,16 +3210,16 @@
         <v>33</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F34" s="8">
         <v>108180</v>
@@ -3254,7 +3255,7 @@
         <v>0.29738346624692302</v>
       </c>
       <c r="Q34" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="R34">
         <v>30</v>
@@ -3263,7 +3264,7 @@
         <v>0</v>
       </c>
       <c r="T34" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:21">
@@ -3271,16 +3272,16 @@
         <v>34</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F35" s="8">
         <v>360231</v>
@@ -3316,7 +3317,7 @@
         <v>0.27047377580896798</v>
       </c>
       <c r="Q35" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="R35">
         <v>36</v>
@@ -3325,7 +3326,7 @@
         <v>0</v>
       </c>
       <c r="T35" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:21">
@@ -3333,16 +3334,16 @@
         <v>35</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F36" s="8">
         <v>358829</v>
@@ -3378,7 +3379,7 @@
         <v>0.761533758381152</v>
       </c>
       <c r="Q36" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="R36">
         <v>37</v>
@@ -3387,7 +3388,7 @@
         <v>0</v>
       </c>
       <c r="T36" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:21">
@@ -3395,16 +3396,16 @@
         <v>36</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F37" s="8">
         <v>190040</v>
@@ -3440,7 +3441,7 @@
         <v>0.73944191330009301</v>
       </c>
       <c r="Q37" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="R37">
         <v>5</v>
@@ -3449,7 +3450,7 @@
         <v>0</v>
       </c>
       <c r="T37" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:21">
@@ -3457,16 +3458,16 @@
         <v>37</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F38" s="8">
         <v>819725</v>
@@ -3502,7 +3503,7 @@
         <v>0.91860621685125998</v>
       </c>
       <c r="Q38" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="R38">
         <v>38</v>
@@ -3511,7 +3512,7 @@
         <v>0</v>
       </c>
       <c r="T38" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="39" spans="1:21">
@@ -3519,16 +3520,16 @@
         <v>38</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F39" s="8">
         <v>2886767</v>
@@ -3564,7 +3565,7 @@
         <v>0.68386541999528505</v>
       </c>
       <c r="Q39" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="R39">
         <v>49</v>
@@ -3573,7 +3574,7 @@
         <v>0</v>
       </c>
       <c r="T39" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="40" spans="1:21">
@@ -3581,16 +3582,16 @@
         <v>39</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F40" s="8">
         <v>268</v>
@@ -3626,7 +3627,7 @@
         <v>0</v>
       </c>
       <c r="Q40" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="R40">
         <v>6</v>
@@ -3635,7 +3636,7 @@
         <v>0</v>
       </c>
       <c r="T40" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:21">
@@ -3643,16 +3644,16 @@
         <v>40</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F41" s="8">
         <v>667038</v>
@@ -3688,7 +3689,7 @@
         <v>0.40943924177721203</v>
       </c>
       <c r="Q41" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="R41">
         <v>39</v>
@@ -3697,7 +3698,7 @@
         <v>0</v>
       </c>
       <c r="T41" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42" spans="1:21">
@@ -3705,16 +3706,16 @@
         <v>41</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F42" s="8">
         <v>468</v>
@@ -3750,7 +3751,7 @@
         <v>0.246110099352886</v>
       </c>
       <c r="Q42" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="R42">
         <v>9</v>
@@ -3759,7 +3760,7 @@
         <v>0</v>
       </c>
       <c r="T42" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:21">
@@ -3767,16 +3768,16 @@
         <v>42</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F43" s="8">
         <v>16736</v>
@@ -3812,7 +3813,7 @@
         <v>1.3417136611662199</v>
       </c>
       <c r="Q43" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="R43">
         <v>51</v>
@@ -3821,7 +3822,7 @@
         <v>0</v>
       </c>
       <c r="T43" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="44" spans="1:21">
@@ -3829,16 +3830,16 @@
         <v>43</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F44" s="8">
         <v>440</v>
@@ -3874,7 +3875,7 @@
         <v>0</v>
       </c>
       <c r="Q44" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="R44">
         <v>31</v>
@@ -3883,7 +3884,7 @@
         <v>0</v>
       </c>
       <c r="T44" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="45" spans="1:21">
@@ -3891,16 +3892,16 @@
         <v>44</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F45" s="8">
         <v>1375</v>
@@ -3936,7 +3937,7 @@
         <v>0.78482742654892701</v>
       </c>
       <c r="Q45" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="R45">
         <v>32</v>
@@ -3945,7 +3946,7 @@
         <v>0</v>
       </c>
       <c r="T45" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="46" spans="1:21">
@@ -3953,16 +3954,16 @@
         <v>45</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F46" s="8">
         <v>28783</v>
@@ -3998,7 +3999,7 @@
         <v>0.85683088484749503</v>
       </c>
       <c r="Q46" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="R46">
         <v>52</v>
@@ -4007,7 +4008,7 @@
         <v>0</v>
       </c>
       <c r="T46" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="47" spans="1:21">
@@ -4015,16 +4016,16 @@
         <v>46</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F47" s="8">
         <v>45628</v>
@@ -4060,7 +4061,7 @@
         <v>1.07619362021107</v>
       </c>
       <c r="Q47" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="R47">
         <v>10</v>
@@ -4069,7 +4070,7 @@
         <v>13</v>
       </c>
       <c r="T47" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="U47"/>
     </row>
@@ -4078,16 +4079,16 @@
         <v>47</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F48" s="8">
         <v>456</v>
@@ -4123,7 +4124,7 @@
         <v>0</v>
       </c>
       <c r="Q48" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="R48">
         <v>60</v>
@@ -4132,7 +4133,7 @@
         <v>0</v>
       </c>
       <c r="T48" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="49" spans="1:21">
@@ -4140,16 +4141,16 @@
         <v>48</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F49" s="8">
         <v>13737</v>
@@ -4185,7 +4186,7 @@
         <v>0.65943230836537003</v>
       </c>
       <c r="Q49" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="R49">
         <v>61</v>
@@ -4194,7 +4195,7 @@
         <v>0</v>
       </c>
       <c r="T49" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="50" spans="1:21">
@@ -4202,16 +4203,16 @@
         <v>49</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F50" s="8">
         <v>2138</v>
@@ -4247,7 +4248,7 @@
         <v>0.56022398725045097</v>
       </c>
       <c r="Q50" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="R50">
         <v>64</v>
@@ -4256,7 +4257,7 @@
         <v>12</v>
       </c>
       <c r="T50" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="U50"/>
     </row>
@@ -4265,16 +4266,16 @@
         <v>50</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F51" s="8">
         <v>10462</v>
@@ -4310,7 +4311,7 @@
         <v>5.4982613128246899E-2</v>
       </c>
       <c r="Q51" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="R51">
         <v>11</v>
@@ -4319,7 +4320,7 @@
         <v>0</v>
       </c>
       <c r="T51" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="52" spans="1:21">
@@ -4327,16 +4328,16 @@
         <v>51</v>
       </c>
       <c r="B52" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="E52" s="8" t="s">
         <v>145</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="E52" s="8" t="s">
-        <v>147</v>
       </c>
       <c r="F52" s="8">
         <v>1263</v>
@@ -4372,7 +4373,7 @@
         <v>0.60647875329127698</v>
       </c>
       <c r="Q52" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="R52">
         <v>14</v>
@@ -4381,7 +4382,7 @@
         <v>0</v>
       </c>
       <c r="T52" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="53" spans="1:21">
@@ -4389,16 +4390,16 @@
         <v>52</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F53" s="8">
         <v>113129</v>
@@ -4434,7 +4435,7 @@
         <v>1.0688591505450999</v>
       </c>
       <c r="Q53" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="R53">
         <v>33</v>
@@ -4443,7 +4444,7 @@
         <v>0</v>
       </c>
       <c r="T53" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="54" spans="1:21">
@@ -4451,16 +4452,16 @@
         <v>53</v>
       </c>
       <c r="B54" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="D54" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="C54" s="8" t="s">
+      <c r="E54" s="8" t="s">
         <v>152</v>
-      </c>
-      <c r="D54" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="E54" s="8" t="s">
-        <v>154</v>
       </c>
       <c r="F54" s="8">
         <v>221555</v>
@@ -4496,7 +4497,7 @@
         <v>0.73222518939546499</v>
       </c>
       <c r="Q54" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="R54">
         <v>50</v>
@@ -4505,7 +4506,7 @@
         <v>0</v>
       </c>
       <c r="T54" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="55" spans="1:21">
@@ -4513,16 +4514,16 @@
         <v>54</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F55" s="8">
         <v>303</v>
@@ -4558,7 +4559,7 @@
         <v>0</v>
       </c>
       <c r="Q55" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="R55">
         <v>65</v>
@@ -4567,7 +4568,7 @@
         <v>0</v>
       </c>
       <c r="T55" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="56" spans="1:21">
@@ -4575,16 +4576,16 @@
         <v>55</v>
       </c>
       <c r="B56" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D56" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="C56" s="8" t="s">
+      <c r="E56" s="8" t="s">
         <v>159</v>
-      </c>
-      <c r="D56" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="E56" s="8" t="s">
-        <v>161</v>
       </c>
       <c r="F56" s="8">
         <v>16585</v>
@@ -4620,7 +4621,7 @@
         <v>0.55833149765035806</v>
       </c>
       <c r="Q56" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="R56">
         <v>62</v>
@@ -4629,7 +4630,7 @@
         <v>0</v>
       </c>
       <c r="T56" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="57" spans="1:21">
@@ -4637,16 +4638,16 @@
         <v>56</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F57" s="8">
         <v>14342</v>
@@ -4682,7 +4683,7 @@
         <v>1.3376407922809399</v>
       </c>
       <c r="Q57" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="R57">
         <v>46</v>
@@ -4691,7 +4692,7 @@
         <v>0</v>
       </c>
       <c r="T57" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="58" spans="1:21">
@@ -4699,16 +4700,16 @@
         <v>57</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F58" s="8">
         <v>47144</v>
@@ -4744,7 +4745,7 @@
         <v>1.56071289630564</v>
       </c>
       <c r="Q58" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="R58">
         <v>47</v>
@@ -4753,7 +4754,7 @@
         <v>0</v>
       </c>
       <c r="T58" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="59" spans="1:21">
@@ -4761,16 +4762,16 @@
         <v>58</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F59" s="8">
         <v>1340</v>
@@ -4806,7 +4807,7 @@
         <v>0.55598368824258104</v>
       </c>
       <c r="Q59" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="R59">
         <v>12</v>
@@ -4815,7 +4816,7 @@
         <v>0</v>
       </c>
       <c r="T59" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="60" spans="1:21">
@@ -4823,16 +4824,16 @@
         <v>59</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E60" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F60" s="8">
         <v>74924</v>
@@ -4868,7 +4869,7 @@
         <v>1.1192458467664399</v>
       </c>
       <c r="Q60" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="R60">
         <v>66</v>
@@ -4877,7 +4878,7 @@
         <v>0</v>
       </c>
       <c r="T60" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="61" spans="1:21">
@@ -4885,16 +4886,16 @@
         <v>60</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E61" s="8" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F61" s="8">
         <v>438756</v>
@@ -4930,7 +4931,7 @@
         <v>0.68548283735082105</v>
       </c>
       <c r="Q61" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="R61">
         <v>63</v>
@@ -4939,7 +4940,7 @@
         <v>0</v>
       </c>
       <c r="T61" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="62" spans="1:21">
@@ -4947,16 +4948,16 @@
         <v>61</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E62" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F62" s="8">
         <v>37028</v>
@@ -4992,7 +4993,7 @@
         <v>1.16522712327528</v>
       </c>
       <c r="Q62" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="R62">
         <v>55</v>
@@ -5001,7 +5002,7 @@
         <v>0</v>
       </c>
       <c r="T62" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="63" spans="1:21">
@@ -5009,16 +5010,16 @@
         <v>62</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E63" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F63" s="8">
         <v>2863</v>
@@ -5054,7 +5055,7 @@
         <v>0.56372578496748404</v>
       </c>
       <c r="Q63" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="R63">
         <v>53</v>
@@ -5063,7 +5064,7 @@
         <v>0</v>
       </c>
       <c r="T63" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="64" spans="1:21">
@@ -5071,16 +5072,16 @@
         <v>63</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F64" s="8">
         <v>180327</v>
@@ -5116,7 +5117,7 @@
         <v>1.2730636426522901</v>
       </c>
       <c r="Q64" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="R64">
         <v>54</v>
@@ -5125,7 +5126,7 @@
         <v>0</v>
       </c>
       <c r="T64" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="65" spans="1:20">
@@ -5133,16 +5134,16 @@
         <v>64</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E65" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F65" s="8">
         <v>689797</v>
@@ -5178,7 +5179,7 @@
         <v>1.43599429113344</v>
       </c>
       <c r="Q65" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="R65">
         <v>67</v>
@@ -5187,7 +5188,7 @@
         <v>0</v>
       </c>
       <c r="T65" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="66" spans="1:20">
@@ -5195,16 +5196,16 @@
         <v>65</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E66" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F66" s="8">
         <v>614105</v>
@@ -5240,7 +5241,7 @@
         <v>1.30374504487619</v>
       </c>
       <c r="Q66" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="R66">
         <v>68</v>
@@ -5249,7 +5250,7 @@
         <v>0</v>
       </c>
       <c r="T66" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="67" spans="1:20">
@@ -5257,16 +5258,16 @@
         <v>66</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E67" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F67" s="8">
         <v>35132</v>
@@ -5302,7 +5303,7 @@
         <v>0.69538103330126999</v>
       </c>
       <c r="Q67" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="R67">
         <v>48</v>
@@ -5311,7 +5312,7 @@
         <v>0</v>
       </c>
       <c r="T67" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="68" spans="1:20">
@@ -5319,16 +5320,16 @@
         <v>67</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E68" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F68" s="8">
         <v>813272</v>
@@ -5364,7 +5365,7 @@
         <v>0.59181362527957904</v>
       </c>
       <c r="Q68" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="R68">
         <v>56</v>
@@ -5373,7 +5374,7 @@
         <v>0</v>
       </c>
       <c r="T68" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="69" spans="1:20">
@@ -5381,16 +5382,16 @@
         <v>68</v>
       </c>
       <c r="B69" s="17" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C69" s="17" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D69" s="17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E69" s="17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F69" s="17">
         <v>104321</v>
@@ -5426,7 +5427,7 @@
         <v>0.87362895059149603</v>
       </c>
       <c r="Q69" s="19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="R69">
         <v>13</v>
@@ -5435,7 +5436,7 @@
         <v>0</v>
       </c>
       <c r="T69" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -5520,7 +5521,7 @@
     <cfRule type="containsText" dxfId="0" priority="12" operator="containsText" text="Extinción acelerada"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>